<commit_message>
Add empirical TDEE calculation from calorie and weight data
- Add Calorie movement type for tracking daily calorie intake
- Implement TDEE calculation with 28-day window and 10-day EMA smoothing
- Handle EMA boundary cases: initialize from first available weight, carry forward on gaps
- Add /api/tdee endpoint with detailed success/error responses
- Display TDEE in header with hover tooltip showing calculation details
- Update test data generator to include calorie entries
- Document TDEE algorithm, constants, and error types in CLAUDE.md

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/test_data.xlsx
+++ b/test_data.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,29 +448,27 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>45361</v>
+        <v>45993</v>
       </c>
       <c r="B2" t="n">
-        <v>180</v>
-      </c>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
+        <v>79.40000000000001</v>
+      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>deadlift</t>
+          <t>bodyweight</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>45301</v>
+        <v>45366</v>
       </c>
       <c r="B3" t="n">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C3" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -480,216 +478,194 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>45363</v>
+        <v>45306</v>
       </c>
       <c r="B4" t="n">
-        <v>75</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>snatch</t>
+          <t>bodyweight</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>45658</v>
+        <v>45982</v>
       </c>
       <c r="B5" t="n">
-        <v>105</v>
-      </c>
-      <c r="C5" t="n">
-        <v>1</v>
-      </c>
+        <v>79.8</v>
+      </c>
+      <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>bench</t>
+          <t>bodyweight</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>45306</v>
+        <v>45995</v>
       </c>
       <c r="B6" t="n">
-        <v>160</v>
-      </c>
-      <c r="C6" t="n">
-        <v>5</v>
-      </c>
+        <v>2549</v>
+      </c>
+      <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>deadlift</t>
+          <t>calorie</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>45303</v>
+        <v>45361</v>
       </c>
       <c r="B7" t="n">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="C7" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>bench</t>
+          <t>deadlift</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>45327</v>
+        <v>45988</v>
       </c>
       <c r="B8" t="n">
-        <v>72</v>
-      </c>
-      <c r="C8" t="n">
-        <v>2</v>
-      </c>
+        <v>79.3</v>
+      </c>
+      <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>snatch</t>
+          <t>bodyweight</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>45332</v>
+        <v>46000</v>
       </c>
       <c r="B9" t="n">
-        <v>95</v>
-      </c>
-      <c r="C9" t="n">
-        <v>3</v>
-      </c>
+        <v>79.59999999999999</v>
+      </c>
+      <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>bench</t>
+          <t>bodyweight</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>45342</v>
+        <v>45968</v>
       </c>
       <c r="B10" t="n">
-        <v>170</v>
-      </c>
-      <c r="C10" t="n">
-        <v>3</v>
-      </c>
+        <v>2250</v>
+      </c>
+      <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
-          <t>deadlift</t>
+          <t>calorie</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>45299</v>
+        <v>45958</v>
       </c>
       <c r="B11" t="n">
-        <v>70</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
-          <t>snatch</t>
+          <t>bodyweight</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>45306</v>
+        <v>45977</v>
       </c>
       <c r="B12" t="n">
-        <v>83</v>
+        <v>2322</v>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
         <is>
-          <t>bodyweight</t>
+          <t>calorie</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>45356</v>
+        <v>45962</v>
       </c>
       <c r="B13" t="n">
-        <v>100</v>
-      </c>
-      <c r="C13" t="n">
-        <v>1</v>
-      </c>
+        <v>2464</v>
+      </c>
+      <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
         <is>
-          <t>bench</t>
+          <t>calorie</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>45363</v>
+        <v>45962</v>
       </c>
       <c r="B14" t="n">
-        <v>100</v>
-      </c>
-      <c r="C14" t="n">
-        <v>1</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr">
         <is>
-          <t>cj</t>
+          <t>bodyweight</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>45311</v>
+        <v>45964</v>
       </c>
       <c r="B15" t="n">
-        <v>135</v>
-      </c>
-      <c r="C15" t="n">
-        <v>3</v>
-      </c>
+        <v>79.90000000000001</v>
+      </c>
+      <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr">
         <is>
-          <t>squat</t>
+          <t>bodyweight</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>45366</v>
+        <v>45995</v>
       </c>
       <c r="B16" t="n">
-        <v>140</v>
-      </c>
-      <c r="C16" t="n">
-        <v>8</v>
-      </c>
+        <v>79.40000000000001</v>
+      </c>
+      <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr">
         <is>
-          <t>squat</t>
+          <t>bodyweight</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>45323</v>
+        <v>45990</v>
       </c>
       <c r="B17" t="n">
-        <v>82</v>
+        <v>79.5</v>
       </c>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr">
@@ -700,90 +676,80 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>45658</v>
+        <v>45994</v>
       </c>
       <c r="B18" t="n">
-        <v>155</v>
-      </c>
-      <c r="C18" t="n">
-        <v>1</v>
-      </c>
+        <v>79.7</v>
+      </c>
+      <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr">
         <is>
-          <t>squat</t>
+          <t>bodyweight</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>45337</v>
+        <v>45975</v>
       </c>
       <c r="B19" t="n">
-        <v>140</v>
-      </c>
-      <c r="C19" t="n">
-        <v>5</v>
-      </c>
+        <v>2216</v>
+      </c>
+      <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr">
         <is>
-          <t>squat</t>
+          <t>calorie</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>45299</v>
+        <v>45987</v>
       </c>
       <c r="B20" t="n">
-        <v>90</v>
-      </c>
-      <c r="C20" t="n">
-        <v>1</v>
-      </c>
+        <v>79.40000000000001</v>
+      </c>
+      <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr">
         <is>
-          <t>cj</t>
+          <t>bodyweight</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>45352</v>
+        <v>45984</v>
       </c>
       <c r="B21" t="n">
-        <v>150</v>
-      </c>
-      <c r="C21" t="n">
-        <v>1</v>
-      </c>
+        <v>79.8</v>
+      </c>
+      <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr">
         <is>
-          <t>squat</t>
+          <t>bodyweight</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>45350</v>
+        <v>45981</v>
       </c>
       <c r="B22" t="n">
-        <v>145</v>
-      </c>
-      <c r="C22" t="n">
-        <v>2</v>
-      </c>
+        <v>79.7</v>
+      </c>
+      <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr">
         <is>
-          <t>squat</t>
+          <t>bodyweight</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>45296</v>
+        <v>45979</v>
       </c>
       <c r="B23" t="n">
-        <v>82.5</v>
+        <v>79.8</v>
       </c>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr">
@@ -794,59 +760,1283 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>45361</v>
+        <v>45976</v>
       </c>
       <c r="B24" t="n">
-        <v>81.5</v>
+        <v>2580</v>
       </c>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr">
         <is>
-          <t>bodyweight</t>
+          <t>calorie</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>45327</v>
+        <v>45974</v>
       </c>
       <c r="B25" t="n">
-        <v>95</v>
-      </c>
-      <c r="C25" t="n">
-        <v>1</v>
-      </c>
+        <v>2410</v>
+      </c>
+      <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr">
         <is>
-          <t>cj</t>
+          <t>calorie</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>45323</v>
-      </c>
-      <c r="B26" t="inlineStr"/>
-      <c r="C26" t="n">
-        <v>5</v>
-      </c>
+        <v>45970</v>
+      </c>
+      <c r="B26" t="n">
+        <v>2570</v>
+      </c>
+      <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr">
         <is>
-          <t>squat</t>
+          <t>calorie</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
+        <v>45972</v>
+      </c>
+      <c r="B27" t="n">
+        <v>2057</v>
+      </c>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>calorie</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>45658</v>
+      </c>
+      <c r="B28" t="n">
+        <v>155</v>
+      </c>
+      <c r="C28" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>squat</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>45350</v>
+      </c>
+      <c r="B29" t="n">
+        <v>145</v>
+      </c>
+      <c r="C29" t="n">
+        <v>2</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>squat</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>45363</v>
+      </c>
+      <c r="B30" t="n">
+        <v>100</v>
+      </c>
+      <c r="C30" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>cj</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>45969</v>
+      </c>
+      <c r="B31" t="n">
+        <v>79.90000000000001</v>
+      </c>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>bodyweight</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>45999</v>
+      </c>
+      <c r="B32" t="n">
+        <v>79.59999999999999</v>
+      </c>
+      <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>bodyweight</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>45965</v>
+      </c>
+      <c r="B33" t="n">
+        <v>79.90000000000001</v>
+      </c>
+      <c r="C33" t="inlineStr"/>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>bodyweight</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>45303</v>
+      </c>
+      <c r="B34" t="n">
+        <v>90</v>
+      </c>
+      <c r="C34" t="n">
+        <v>5</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>bench</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>45998</v>
+      </c>
+      <c r="B35" t="n">
+        <v>79.59999999999999</v>
+      </c>
+      <c r="C35" t="inlineStr"/>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>bodyweight</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>45971</v>
+      </c>
+      <c r="B36" t="n">
+        <v>2332</v>
+      </c>
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>calorie</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>45993</v>
+      </c>
+      <c r="B37" t="n">
+        <v>2011</v>
+      </c>
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>calorie</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>45966</v>
+      </c>
+      <c r="B38" t="n">
+        <v>2073</v>
+      </c>
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>calorie</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>45311</v>
+      </c>
+      <c r="B39" t="n">
+        <v>135</v>
+      </c>
+      <c r="C39" t="n">
+        <v>3</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>squat</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>45973</v>
+      </c>
+      <c r="B40" t="n">
+        <v>80</v>
+      </c>
+      <c r="C40" t="inlineStr"/>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>bodyweight</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>46000</v>
+      </c>
+      <c r="B41" t="n">
+        <v>2182</v>
+      </c>
+      <c r="C41" t="inlineStr"/>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>calorie</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>45992</v>
+      </c>
+      <c r="B42" t="n">
+        <v>79.7</v>
+      </c>
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>bodyweight</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>45999</v>
+      </c>
+      <c r="B43" t="n">
+        <v>2269</v>
+      </c>
+      <c r="C43" t="inlineStr"/>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>calorie</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>45974</v>
+      </c>
+      <c r="B44" t="n">
+        <v>79.8</v>
+      </c>
+      <c r="C44" t="inlineStr"/>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>bodyweight</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>45991</v>
+      </c>
+      <c r="B45" t="n">
+        <v>79.7</v>
+      </c>
+      <c r="C45" t="inlineStr"/>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>bodyweight</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>45984</v>
+      </c>
+      <c r="B46" t="n">
+        <v>2224</v>
+      </c>
+      <c r="C46" t="inlineStr"/>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>calorie</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45979</v>
+      </c>
+      <c r="B47" t="n">
+        <v>2469</v>
+      </c>
+      <c r="C47" t="inlineStr"/>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>calorie</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>45997</v>
+      </c>
+      <c r="B48" t="n">
+        <v>79.5</v>
+      </c>
+      <c r="C48" t="inlineStr"/>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>bodyweight</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>45968</v>
+      </c>
+      <c r="B49" t="n">
+        <v>80</v>
+      </c>
+      <c r="C49" t="inlineStr"/>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>bodyweight</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>45658</v>
+      </c>
+      <c r="B50" t="n">
+        <v>105</v>
+      </c>
+      <c r="C50" t="n">
+        <v>1</v>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>bench</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>45971</v>
+      </c>
+      <c r="B51" t="n">
+        <v>79.7</v>
+      </c>
+      <c r="C51" t="inlineStr"/>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>bodyweight</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>45972</v>
+      </c>
+      <c r="B52" t="n">
+        <v>79.90000000000001</v>
+      </c>
+      <c r="C52" t="inlineStr"/>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>bodyweight</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>45363</v>
+      </c>
+      <c r="B53" t="n">
+        <v>75</v>
+      </c>
+      <c r="C53" t="n">
+        <v>1</v>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>snatch</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>45964</v>
+      </c>
+      <c r="B54" t="n">
+        <v>2363</v>
+      </c>
+      <c r="C54" t="inlineStr"/>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>calorie</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>45301</v>
+      </c>
+      <c r="B55" t="n">
+        <v>130</v>
+      </c>
+      <c r="C55" t="n">
+        <v>5</v>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>squat</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>45956</v>
+      </c>
+      <c r="B56" t="n">
+        <v>80</v>
+      </c>
+      <c r="C56" t="inlineStr"/>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>bodyweight</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>45352</v>
+      </c>
+      <c r="B57" t="n">
+        <v>150</v>
+      </c>
+      <c r="C57" t="n">
+        <v>1</v>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>squat</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>45966</v>
+      </c>
+      <c r="B58" t="n">
+        <v>79.90000000000001</v>
+      </c>
+      <c r="C58" t="inlineStr"/>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>bodyweight</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>45980</v>
+      </c>
+      <c r="B59" t="n">
+        <v>2142</v>
+      </c>
+      <c r="C59" t="inlineStr"/>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>calorie</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>45978</v>
+      </c>
+      <c r="B60" t="n">
+        <v>79.7</v>
+      </c>
+      <c r="C60" t="inlineStr"/>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>bodyweight</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
         <v>45323</v>
       </c>
-      <c r="B27" t="n">
+      <c r="B61" t="n">
+        <v>82</v>
+      </c>
+      <c r="C61" t="inlineStr"/>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>bodyweight</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>45983</v>
+      </c>
+      <c r="B62" t="n">
+        <v>79.7</v>
+      </c>
+      <c r="C62" t="inlineStr"/>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>bodyweight</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>45299</v>
+      </c>
+      <c r="B63" t="n">
+        <v>70</v>
+      </c>
+      <c r="C63" t="n">
+        <v>1</v>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>snatch</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>45970</v>
+      </c>
+      <c r="B64" t="n">
+        <v>79.7</v>
+      </c>
+      <c r="C64" t="inlineStr"/>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>bodyweight</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>45976</v>
+      </c>
+      <c r="B65" t="n">
+        <v>79.90000000000001</v>
+      </c>
+      <c r="C65" t="inlineStr"/>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>bodyweight</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>45977</v>
+      </c>
+      <c r="B66" t="n">
+        <v>79.5</v>
+      </c>
+      <c r="C66" t="inlineStr"/>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>bodyweight</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>45356</v>
+      </c>
+      <c r="B67" t="n">
         <v>100</v>
       </c>
-      <c r="C27" t="n">
+      <c r="C67" t="n">
+        <v>1</v>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>bench</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>45980</v>
+      </c>
+      <c r="B68" t="n">
+        <v>79.90000000000001</v>
+      </c>
+      <c r="C68" t="inlineStr"/>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>bodyweight</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>45982</v>
+      </c>
+      <c r="B69" t="n">
+        <v>2598</v>
+      </c>
+      <c r="C69" t="inlineStr"/>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>calorie</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>45991</v>
+      </c>
+      <c r="B70" t="n">
+        <v>2479</v>
+      </c>
+      <c r="C70" t="inlineStr"/>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>calorie</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>45965</v>
+      </c>
+      <c r="B71" t="n">
+        <v>2273</v>
+      </c>
+      <c r="C71" t="inlineStr"/>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>calorie</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>45981</v>
+      </c>
+      <c r="B72" t="n">
+        <v>2574</v>
+      </c>
+      <c r="C72" t="inlineStr"/>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>calorie</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>45299</v>
+      </c>
+      <c r="B73" t="n">
+        <v>90</v>
+      </c>
+      <c r="C73" t="n">
+        <v>1</v>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>cj</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>45990</v>
+      </c>
+      <c r="B74" t="n">
+        <v>2394</v>
+      </c>
+      <c r="C74" t="inlineStr"/>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>calorie</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>45975</v>
+      </c>
+      <c r="B75" t="n">
+        <v>79.8</v>
+      </c>
+      <c r="C75" t="inlineStr"/>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>bodyweight</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>45985</v>
+      </c>
+      <c r="B76" t="n">
+        <v>2141</v>
+      </c>
+      <c r="C76" t="inlineStr"/>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>calorie</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>45327</v>
+      </c>
+      <c r="B77" t="n">
+        <v>95</v>
+      </c>
+      <c r="C77" t="n">
+        <v>1</v>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>cj</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>45296</v>
+      </c>
+      <c r="B78" t="n">
+        <v>82.5</v>
+      </c>
+      <c r="C78" t="inlineStr"/>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>bodyweight</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>45996</v>
+      </c>
+      <c r="B79" t="n">
+        <v>2348</v>
+      </c>
+      <c r="C79" t="inlineStr"/>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>calorie</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>45989</v>
+      </c>
+      <c r="B80" t="n">
+        <v>2432</v>
+      </c>
+      <c r="C80" t="inlineStr"/>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>calorie</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>45989</v>
+      </c>
+      <c r="B81" t="n">
+        <v>79.5</v>
+      </c>
+      <c r="C81" t="inlineStr"/>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>bodyweight</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>45994</v>
+      </c>
+      <c r="B82" t="n">
+        <v>2117</v>
+      </c>
+      <c r="C82" t="inlineStr"/>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>calorie</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>45985</v>
+      </c>
+      <c r="B83" t="n">
+        <v>79.5</v>
+      </c>
+      <c r="C83" t="inlineStr"/>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>bodyweight</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>45988</v>
+      </c>
+      <c r="B84" t="n">
+        <v>2163</v>
+      </c>
+      <c r="C84" t="inlineStr"/>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>calorie</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>45957</v>
+      </c>
+      <c r="B85" t="n">
+        <v>80</v>
+      </c>
+      <c r="C85" t="inlineStr"/>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>bodyweight</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>45963</v>
+      </c>
+      <c r="B86" t="n">
+        <v>2373</v>
+      </c>
+      <c r="C86" t="inlineStr"/>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>calorie</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="n">
+        <v>45983</v>
+      </c>
+      <c r="B87" t="n">
+        <v>2597</v>
+      </c>
+      <c r="C87" t="inlineStr"/>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>calorie</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="n">
+        <v>45969</v>
+      </c>
+      <c r="B88" t="n">
+        <v>2388</v>
+      </c>
+      <c r="C88" t="inlineStr"/>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>calorie</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="n">
+        <v>45996</v>
+      </c>
+      <c r="B89" t="n">
+        <v>79.5</v>
+      </c>
+      <c r="C89" t="inlineStr"/>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>bodyweight</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n">
+        <v>45961</v>
+      </c>
+      <c r="B90" t="n">
+        <v>79.7</v>
+      </c>
+      <c r="C90" t="inlineStr"/>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>bodyweight</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="n">
+        <v>45959</v>
+      </c>
+      <c r="B91" t="n">
+        <v>80.09999999999999</v>
+      </c>
+      <c r="C91" t="inlineStr"/>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>bodyweight</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="n">
+        <v>45987</v>
+      </c>
+      <c r="B92" t="n">
+        <v>2112</v>
+      </c>
+      <c r="C92" t="inlineStr"/>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>calorie</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="n">
+        <v>45998</v>
+      </c>
+      <c r="B93" t="n">
+        <v>2003</v>
+      </c>
+      <c r="C93" t="inlineStr"/>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>calorie</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n">
+        <v>45337</v>
+      </c>
+      <c r="B94" t="n">
+        <v>140</v>
+      </c>
+      <c r="C94" t="n">
         <v>5</v>
       </c>
-      <c r="D27" t="inlineStr">
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>squat</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="n">
+        <v>45986</v>
+      </c>
+      <c r="B95" t="n">
+        <v>79.8</v>
+      </c>
+      <c r="C95" t="inlineStr"/>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>bodyweight</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="n">
+        <v>45967</v>
+      </c>
+      <c r="B96" t="n">
+        <v>2175</v>
+      </c>
+      <c r="C96" t="inlineStr"/>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>calorie</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>45332</v>
+      </c>
+      <c r="B97" t="n">
+        <v>95</v>
+      </c>
+      <c r="C97" t="n">
+        <v>3</v>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>bench</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n">
+        <v>45961</v>
+      </c>
+      <c r="B98" t="n">
+        <v>2103</v>
+      </c>
+      <c r="C98" t="inlineStr"/>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>calorie</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>45992</v>
+      </c>
+      <c r="B99" t="n">
+        <v>2566</v>
+      </c>
+      <c r="C99" t="inlineStr"/>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>calorie</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>45978</v>
+      </c>
+      <c r="B100" t="n">
+        <v>2511</v>
+      </c>
+      <c r="C100" t="inlineStr"/>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>calorie</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
+        <v>45306</v>
+      </c>
+      <c r="B101" t="n">
+        <v>160</v>
+      </c>
+      <c r="C101" t="n">
+        <v>5</v>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>deadlift</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="n">
+        <v>45997</v>
+      </c>
+      <c r="B102" t="n">
+        <v>2445</v>
+      </c>
+      <c r="C102" t="inlineStr"/>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>calorie</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="n">
+        <v>45327</v>
+      </c>
+      <c r="B103" t="n">
+        <v>72</v>
+      </c>
+      <c r="C103" t="n">
+        <v>2</v>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>snatch</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="n">
+        <v>45960</v>
+      </c>
+      <c r="B104" t="n">
+        <v>79.90000000000001</v>
+      </c>
+      <c r="C104" t="inlineStr"/>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>bodyweight</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="n">
+        <v>45963</v>
+      </c>
+      <c r="B105" t="n">
+        <v>79.90000000000001</v>
+      </c>
+      <c r="C105" t="inlineStr"/>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>bodyweight</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>45967</v>
+      </c>
+      <c r="B106" t="n">
+        <v>80.09999999999999</v>
+      </c>
+      <c r="C106" t="inlineStr"/>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>bodyweight</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="n">
+        <v>45986</v>
+      </c>
+      <c r="B107" t="n">
+        <v>2093</v>
+      </c>
+      <c r="C107" t="inlineStr"/>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>calorie</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="n">
+        <v>45361</v>
+      </c>
+      <c r="B108" t="n">
+        <v>81.5</v>
+      </c>
+      <c r="C108" t="inlineStr"/>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>bodyweight</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="n">
+        <v>45342</v>
+      </c>
+      <c r="B109" t="n">
+        <v>170</v>
+      </c>
+      <c r="C109" t="n">
+        <v>3</v>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>deadlift</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="n">
+        <v>45973</v>
+      </c>
+      <c r="B110" t="n">
+        <v>2032</v>
+      </c>
+      <c r="C110" t="inlineStr"/>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>calorie</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="n">
+        <v>45323</v>
+      </c>
+      <c r="B111" t="inlineStr"/>
+      <c r="C111" t="n">
+        <v>5</v>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>squat</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="n">
+        <v>45323</v>
+      </c>
+      <c r="B112" t="n">
+        <v>100</v>
+      </c>
+      <c r="C112" t="n">
+        <v>5</v>
+      </c>
+      <c r="D112" t="inlineStr">
         <is>
           <t>unknown_movement</t>
         </is>

</xml_diff>